<commit_message>
add service delivery example
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_diabetes.xlsx
+++ b/tests/frameworks/framework_diabetes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/frameworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1DCFE529-61AF-8948-937F-5FD5B7C23C8D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0378834E-693B-EF49-8D4A-A68398D1338A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="19500" windowHeight="11200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19500" windowHeight="11200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="2" r:id="rId1"/>
@@ -1898,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2285,8 +2285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2517,14 +2517,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>

</xml_diff>